<commit_message>
[Adjustements] - Fix tests, add redis, composer.json, cnfigs.
</commit_message>
<xml_diff>
--- a/Teste-excel-laravel.xlsx
+++ b/Teste-excel-laravel.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -37,9 +37,6 @@
     <t xml:space="preserve">cns</t>
   </si>
   <si>
-    <t xml:space="preserve">image_patient</t>
-  </si>
-  <si>
     <t xml:space="preserve">zip_code</t>
   </si>
   <si>
@@ -83,6 +80,9 @@
   </si>
   <si>
     <t xml:space="preserve">CE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null</t>
   </si>
   <si>
     <t xml:space="preserve">Jorge Assunção</t>
@@ -158,10 +158,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -182,6 +183,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -226,8 +232,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -248,22 +262,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
+      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="15.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -303,34 +317,34 @@
       <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>32162</v>
+      <c r="C2" s="1" t="n">
+        <v>36840</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>77824813843</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2" s="0" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" s="0" t="n">
-        <v>12</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>18</v>
@@ -349,8 +363,8 @@
       <c r="B3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>32194</v>
+      <c r="C3" s="1" t="n">
+        <v>36537</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>63235723897</v>
@@ -358,23 +372,26 @@
       <c r="E3" s="0" t="s">
         <v>23</v>
       </c>
+      <c r="F3" s="0" t="s">
+        <v>24</v>
+      </c>
       <c r="G3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <v>10</v>
       </c>
+      <c r="I3" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="J3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="0" t="s">
         <v>28</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,8 +401,8 @@
       <c r="B4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>32224</v>
+      <c r="C4" s="1" t="n">
+        <v>36818</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>52115828615</v>
@@ -393,23 +410,26 @@
       <c r="E4" s="0" t="s">
         <v>31</v>
       </c>
+      <c r="F4" s="0" t="s">
+        <v>32</v>
+      </c>
       <c r="G4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <v>158</v>
       </c>
+      <c r="I4" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="J4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="L4" s="0" t="s">
         <v>36</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -419,8 +439,8 @@
       <c r="B5" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>32896</v>
+      <c r="C5" s="1" t="n">
+        <v>36793</v>
       </c>
       <c r="D5" s="0" t="n">
         <v>44962574671</v>
@@ -428,23 +448,26 @@
       <c r="E5" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="F5" s="0" t="s">
+        <v>40</v>
+      </c>
       <c r="G5" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>1010</v>
       </c>
+      <c r="I5" s="0" t="s">
+        <v>34</v>
+      </c>
       <c r="J5" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="0" t="s">
         <v>43</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Excel] Adjustement ins excel for import.
</commit_message>
<xml_diff>
--- a/Teste-excel-laravel.xlsx
+++ b/Teste-excel-laravel.xlsx
@@ -160,9 +160,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -183,11 +183,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -232,7 +227,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -241,7 +236,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -265,13 +264,14 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L8" activeCellId="0" sqref="L8"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="23.23"/>
@@ -287,7 +287,7 @@
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
@@ -325,7 +325,7 @@
       <c r="B2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="n">
+      <c r="C2" s="2" t="n">
         <v>36840</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -363,7 +363,7 @@
       <c r="B3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="2" t="n">
         <v>36537</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -390,7 +390,7 @@
       <c r="K3" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -401,7 +401,7 @@
       <c r="B4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="1" t="n">
+      <c r="C4" s="2" t="n">
         <v>36818</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -428,7 +428,7 @@
       <c r="K4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -439,7 +439,7 @@
       <c r="B5" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="1" t="n">
+      <c r="C5" s="2" t="n">
         <v>36793</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -466,14 +466,14 @@
       <c r="K5" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="3" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>

</xml_diff>